<commit_message>
updated bonus task solution
</commit_message>
<xml_diff>
--- a/Lecture04_bonus.xlsx
+++ b/Lecture04_bonus.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6566985eb95ae6f7/SkillBox/Новая программа обучения/Знакомство с базами данных/Лекция 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\OneDrive\Documents\Private\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{9053F05F-A5C0-6D47-8331-9840CFEBE842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CB3FED5-6C4D-F149-BC63-1A620995ABFF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{A7129D13-117F-2E48-871A-A287849D6CCE}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Библиотека Структура таблиц" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="76">
   <si>
     <t>Параметр</t>
   </si>
@@ -88,9 +87,6 @@
     <t>Дата рождения</t>
   </si>
   <si>
-    <t>Отчетсво</t>
-  </si>
-  <si>
     <t>Passport_ser</t>
   </si>
   <si>
@@ -121,12 +117,6 @@
     <t>Pages</t>
   </si>
   <si>
-    <t>Reader_id</t>
-  </si>
-  <si>
-    <t>Уникальный идентификатор  книги</t>
-  </si>
-  <si>
     <t>Название книги</t>
   </si>
   <si>
@@ -169,18 +159,12 @@
     <t>Position</t>
   </si>
   <si>
-    <t>Empl_id</t>
-  </si>
-  <si>
     <t>Уникальный идентификатор Сотрудника</t>
   </si>
   <si>
     <t>Style_ID</t>
   </si>
   <si>
-    <t>Уникальный идентификатор  жанра</t>
-  </si>
-  <si>
     <t>Название жанра</t>
   </si>
   <si>
@@ -197,12 +181,90 @@
   </si>
   <si>
     <t>Style_id</t>
+  </si>
+  <si>
+    <t>Имя сотрудника</t>
+  </si>
+  <si>
+    <t>Отчество</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Event_ID</t>
+  </si>
+  <si>
+    <t>Дата выдачи</t>
+  </si>
+  <si>
+    <t>rent_date</t>
+  </si>
+  <si>
+    <t>return_date</t>
+  </si>
+  <si>
+    <t>Дата возврата</t>
+  </si>
+  <si>
+    <t>Уникальный идентификатор события</t>
+  </si>
+  <si>
+    <t>Журнал событий</t>
+  </si>
+  <si>
+    <t>Уникальный идентификатор книги</t>
+  </si>
+  <si>
+    <t>Уникальный идентификатор жанра</t>
+  </si>
+  <si>
+    <t>Уникальный идентификатор автора</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Уникальный идентификатор происхождения</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>Состояние</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Телефон</t>
+  </si>
+  <si>
+    <t>Уникальный идентификатор состояния</t>
+  </si>
+  <si>
+    <t>state_id</t>
+  </si>
+  <si>
+    <t>Происхождение</t>
+  </si>
+  <si>
+    <t>origin</t>
+  </si>
+  <si>
+    <t>origin_id</t>
+  </si>
+  <si>
+    <t>Origin_id</t>
+  </si>
+  <si>
+    <t>страна происхождения</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -254,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -582,11 +644,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
@@ -616,9 +761,17 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -637,23 +790,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2540000</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>116418</xdr:rowOff>
+      <xdr:rowOff>116419</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>111241</xdr:rowOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="2" name="Прямая соединительная линия 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C79DCE6-5CEF-1243-A529-ABB456F214B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C79DCE6-5CEF-1243-A529-ABB456F214B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -661,8 +814,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5960657" y="876564"/>
-          <a:ext cx="7082336" cy="1635626"/>
+          <a:off x="12382500" y="868894"/>
+          <a:ext cx="419100" cy="378881"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -692,23 +845,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>18540</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>92700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1653</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>84667</xdr:rowOff>
+      <xdr:rowOff>84668</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="3" name="Прямая соединительная линия 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E170005A-45D6-B541-BF26-B09DAB81B24D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E170005A-45D6-B541-BF26-B09DAB81B24D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -716,8 +869,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6007007" y="2706861"/>
-          <a:ext cx="7037639" cy="1373207"/>
+          <a:off x="12382500" y="1466850"/>
+          <a:ext cx="420753" cy="2561168"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -763,7 +916,7 @@
         <xdr:cNvPr id="6" name="Прямая соединительная линия 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20AC2CF9-8BF0-1649-B4FD-24EEF4E87697}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{20AC2CF9-8BF0-1649-B4FD-24EEF4E87697}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -818,7 +971,7 @@
         <xdr:cNvPr id="9" name="Прямая соединительная линия 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5883CA3-DC0E-7045-8D88-5F4E2052F4D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5883CA3-DC0E-7045-8D88-5F4E2052F4D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -873,7 +1026,7 @@
         <xdr:cNvPr id="13" name="Прямая соединительная линия 12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749E119D-5113-DE4C-83FC-1471B26716DF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{749E119D-5113-DE4C-83FC-1471B26716DF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -928,7 +1081,7 @@
         <xdr:cNvPr id="14" name="Прямая соединительная линия 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E37C41E-2D94-CA42-BAF9-76BAF25AADBB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{4E37C41E-2D94-CA42-BAF9-76BAF25AADBB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -983,7 +1136,7 @@
         <xdr:cNvPr id="15" name="Прямая соединительная линия 14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAAEF33D-5D5F-E94D-8194-CDD20ADEFA43}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CAAEF33D-5D5F-E94D-8194-CDD20ADEFA43}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1038,7 +1191,7 @@
         <xdr:cNvPr id="16" name="Прямая соединительная линия 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9887541C-BE8F-6B49-8755-B5C2E41E1B1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9887541C-BE8F-6B49-8755-B5C2E41E1B1D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1093,7 +1246,7 @@
         <xdr:cNvPr id="21" name="Прямая соединительная линия 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C619C77-0DEE-D844-8EF8-BC6875200131}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C619C77-0DEE-D844-8EF8-BC6875200131}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1103,6 +1256,446 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="518583" y="1873250"/>
           <a:ext cx="10584" cy="2215547"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571502</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Прямая соединительная линия 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C619C77-0DEE-D844-8EF8-BC6875200131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="561975" y="4429125"/>
+          <a:ext cx="9527" cy="1333501"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>565150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>79376</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>836083</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Прямая соединительная линия 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{749E119D-5113-DE4C-83FC-1471B26716DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="565150" y="5775326"/>
+          <a:ext cx="270933" cy="6349"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4233</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Прямая соединительная линия 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{749E119D-5113-DE4C-83FC-1471B26716DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="590550" y="4429125"/>
+          <a:ext cx="270933" cy="6349"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>3067050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="23" name="Прямая соединительная линия 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C79DCE6-5CEF-1243-A529-ABB456F214B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6534150" y="857251"/>
+          <a:ext cx="676275" cy="228599"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Прямая соединительная линия 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2C79DCE6-5CEF-1243-A529-ABB456F214B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6391275" y="5819775"/>
+          <a:ext cx="523875" cy="838200"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>332317</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>100280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>504190</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>106629</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="28" name="Прямая соединительная линия 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{A5883CA3-DC0E-7045-8D88-5F4E2052F4D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6714067" y="2052905"/>
+          <a:ext cx="171873" cy="6349"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>327025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>121447</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>491278</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127796</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Прямая соединительная линия 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{749E119D-5113-DE4C-83FC-1471B26716DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6708775" y="4064797"/>
+          <a:ext cx="164253" cy="6349"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FFC000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>328083</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="30" name="Прямая соединительная линия 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8C619C77-0DEE-D844-8EF8-BC6875200131}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6709833" y="2025650"/>
+          <a:ext cx="5292" cy="2070100"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1429,31 +2022,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F59128E-9A4E-D545-8CD0-55E8BECFFA9F}">
-  <dimension ref="A1:AJ90"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AI90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="137" zoomScaleNormal="137" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="33.6640625" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" customWidth="1"/>
-    <col min="12" max="12" width="5.83203125" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7" customWidth="1"/>
-    <col min="15" max="15" width="7.83203125" customWidth="1"/>
-    <col min="16" max="16" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.09765625" customWidth="1"/>
+    <col min="2" max="2" width="15.19921875" customWidth="1"/>
+    <col min="3" max="3" width="10.19921875" customWidth="1"/>
+    <col min="4" max="4" width="8.69921875" customWidth="1"/>
+    <col min="5" max="5" width="40.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.796875" customWidth="1"/>
+    <col min="7" max="7" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.796875" customWidth="1"/>
+    <col min="12" max="12" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7" customWidth="1"/>
+    <col min="14" max="14" width="7.796875" customWidth="1"/>
+    <col min="15" max="15" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1489,29 +2084,30 @@
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
-      <c r="AJ1" s="1"/>
-    </row>
-    <row r="2" spans="1:36" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:35" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1"/>
       <c r="B2" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="G2" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
       <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="22" t="s">
-        <v>38</v>
-      </c>
+      <c r="L2" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
+      <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -1531,9 +2127,8 @@
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-    </row>
-    <row r="3" spans="1:36" ht="22" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:35" ht="21.6" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="23" t="s">
         <v>0</v>
@@ -1548,25 +2143,33 @@
         <v>3</v>
       </c>
       <c r="F3" s="6"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="26" t="s">
+      <c r="G3" s="23" t="s">
         <v>0</v>
       </c>
+      <c r="H3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="35"/>
+      <c r="L3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="N3" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="28" t="s">
+      <c r="O3" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="Q3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -1585,12 +2188,11 @@
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
-      <c r="AJ3" s="1"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>9</v>
@@ -1599,28 +2201,36 @@
         <v>10</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F4" s="6"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="G4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="9">
+      <c r="I4" s="9">
         <v>10</v>
       </c>
-      <c r="P4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q4" s="3"/>
+      <c r="J4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="35"/>
+      <c r="L4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N4" s="9">
+        <v>10</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -1639,9 +2249,8 @@
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" s="8" t="s">
         <v>5</v>
@@ -1653,28 +2262,36 @@
         <v>100</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F5" s="6"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="11" t="s">
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="9">
+        <v>10</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="35"/>
+      <c r="L5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O5" s="9">
+      <c r="N5" s="9">
         <v>30</v>
       </c>
-      <c r="P5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q5" s="3"/>
+      <c r="O5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
@@ -1693,12 +2310,11 @@
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>9</v>
@@ -1707,28 +2323,36 @@
         <v>10</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F6" s="6"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="11" t="s">
+      <c r="G6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="9">
+        <v>10</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="35"/>
+      <c r="L6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="9">
+      <c r="N6" s="9">
         <v>30</v>
       </c>
-      <c r="P6" s="12" t="s">
+      <c r="O6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="Q6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
@@ -1747,9 +2371,8 @@
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="8" t="s">
         <v>6</v>
@@ -1764,25 +2387,33 @@
         <v>7</v>
       </c>
       <c r="F7" s="6"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="11" t="s">
+      <c r="G7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="9">
+        <v>10</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K7" s="35"/>
+      <c r="L7" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O7" s="9">
+      <c r="N7" s="9">
         <v>30</v>
       </c>
-      <c r="P7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q7" s="3"/>
+      <c r="O7" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
@@ -1801,12 +2432,11 @@
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="8" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>11</v>
@@ -1815,28 +2445,36 @@
         <v>8</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F8" s="6"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="11" t="s">
+      <c r="G8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="9">
+        <v>12</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K8" s="35"/>
+      <c r="L8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N8" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="9">
+      <c r="N8" s="9">
         <v>8</v>
       </c>
-      <c r="P8" s="12" t="s">
+      <c r="O8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Q8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
@@ -1855,12 +2493,11 @@
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" s="8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>9</v>
@@ -1869,28 +2506,36 @@
         <v>10</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9" s="6"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="9" t="s">
+      <c r="G9" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="9">
+        <v>12</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="35"/>
+      <c r="L9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O9" s="9">
+      <c r="N9" s="9">
         <v>10</v>
       </c>
-      <c r="P9" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" s="3"/>
+      <c r="O9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
@@ -1909,12 +2554,11 @@
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2"/>
       <c r="B10" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>9</v>
@@ -1926,25 +2570,33 @@
         <v>1</v>
       </c>
       <c r="F10" s="6"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="11" t="s">
+      <c r="G10" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I10" s="20">
+        <v>10</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="K10" s="35"/>
+      <c r="L10" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="9">
         <v>20</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="O10" s="9">
+      <c r="O10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="P10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
@@ -1963,12 +2615,11 @@
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-    </row>
-    <row r="11" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>8</v>
@@ -1977,28 +2628,28 @@
         <v>10</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F11" s="6"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="O11" s="14">
-        <v>1</v>
-      </c>
-      <c r="P11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q11" s="3"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="M11" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="N11" s="33">
+        <v>10</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
@@ -2017,33 +2668,32 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-    </row>
-    <row r="12" spans="1:36" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2"/>
-      <c r="B12" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="17">
-        <v>10</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>37</v>
-      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="10"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="18"/>
-      <c r="N12" s="18"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
+      <c r="L12" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N12" s="14">
+        <v>1</v>
+      </c>
+      <c r="O12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
@@ -2063,33 +2713,24 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:35" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
-      <c r="B13" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="9">
-        <v>10</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>46</v>
-      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
-      <c r="P13" s="5"/>
+      <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
@@ -2109,25 +2750,24 @@
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-    </row>
-    <row r="14" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="19"/>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="21"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
-      <c r="P14" s="5"/>
+      <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
@@ -2147,9 +2787,8 @@
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
-    </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>
@@ -2165,7 +2804,7 @@
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
+      <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
@@ -2185,9 +2824,8 @@
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
-      <c r="AJ15" s="1"/>
-    </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -2203,7 +2841,7 @@
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
-      <c r="P16" s="5"/>
+      <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
@@ -2223,29 +2861,30 @@
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
-      <c r="AJ16" s="1"/>
-    </row>
-    <row r="17" spans="1:36" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:35" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="22" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="G17" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
       <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="22" t="s">
-        <v>41</v>
-      </c>
+      <c r="L17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
-      <c r="P17" s="4"/>
+      <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -2265,9 +2904,8 @@
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-    </row>
-    <row r="18" spans="1:36" ht="22" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:35" ht="21.6" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A18" s="2"/>
       <c r="B18" s="23" t="s">
         <v>0</v>
@@ -2282,24 +2920,32 @@
         <v>3</v>
       </c>
       <c r="F18" s="6"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="G18" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="26" t="s">
+      <c r="L18" s="26" t="s">
         <v>0</v>
       </c>
+      <c r="M18" s="27" t="s">
+        <v>1</v>
+      </c>
       <c r="N18" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="O18" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="P18" s="28" t="s">
+      <c r="O18" s="28" t="s">
         <v>3</v>
       </c>
+      <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
@@ -2319,12 +2965,11 @@
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
-    </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="8" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>9</v>
@@ -2333,27 +2978,35 @@
         <v>10</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="F19" s="6"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="G19" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="9">
+        <v>10</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>69</v>
+      </c>
       <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="11" t="s">
+      <c r="L19" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="M19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="N19" s="9">
+        <v>10</v>
+      </c>
+      <c r="O19" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="O19" s="9">
-        <v>10</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>46</v>
-      </c>
+      <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
@@ -2373,9 +3026,8 @@
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
-      <c r="AJ19" s="1"/>
-    </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2"/>
       <c r="B20" s="8" t="s">
         <v>5</v>
@@ -2387,27 +3039,35 @@
         <v>100</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="F20" s="6"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="G20" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="I20" s="20">
+        <v>100</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>66</v>
+      </c>
       <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="11" t="s">
+      <c r="L20" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N20" s="9" t="s">
+      <c r="M20" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="9">
+      <c r="N20" s="9">
         <v>30</v>
       </c>
-      <c r="P20" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="O20" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
@@ -2427,12 +3087,11 @@
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
-      <c r="AJ20" s="1"/>
-    </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>9</v>
@@ -2441,27 +3100,27 @@
         <v>10</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="F21" s="6"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
       <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="11" t="s">
+      <c r="L21" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N21" s="9" t="s">
+      <c r="M21" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O21" s="9">
+      <c r="N21" s="9">
         <v>30</v>
       </c>
-      <c r="P21" s="12" t="s">
+      <c r="O21" s="12" t="s">
         <v>14</v>
       </c>
+      <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
@@ -2481,9 +3140,8 @@
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
-      <c r="AJ21" s="1"/>
-    </row>
-    <row r="22" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2"/>
       <c r="B22" s="19" t="s">
         <v>6</v>
@@ -2503,19 +3161,19 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="11" t="s">
+      <c r="L22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="N22" s="9" t="s">
+      <c r="M22" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O22" s="9">
+      <c r="N22" s="9">
         <v>30</v>
       </c>
-      <c r="P22" s="12" t="s">
-        <v>18</v>
-      </c>
+      <c r="O22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="P22" s="1"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -2535,9 +3193,8 @@
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
-      <c r="AJ22" s="1"/>
-    </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="18"/>
       <c r="C23" s="18"/>
@@ -2549,19 +3206,19 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="11" t="s">
+      <c r="L23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="N23" s="9" t="s">
+      <c r="M23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O23" s="9">
+      <c r="N23" s="9">
         <v>8</v>
       </c>
-      <c r="P23" s="12" t="s">
+      <c r="O23" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="P23" s="1"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
@@ -2581,9 +3238,8 @@
       <c r="AG23" s="1"/>
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
-      <c r="AJ23" s="1"/>
-    </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
@@ -2595,19 +3251,19 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="N24" s="9" t="s">
+      <c r="L24" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="M24" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O24" s="9">
+      <c r="N24" s="9">
         <v>10</v>
       </c>
-      <c r="P24" s="12" t="s">
-        <v>22</v>
-      </c>
+      <c r="O24" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
@@ -2627,35 +3283,36 @@
       <c r="AG24" s="1"/>
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
-      <c r="AJ24" s="1"/>
-    </row>
-    <row r="25" spans="1:36" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:35" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
       <c r="B25" s="22" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="6"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
+      <c r="G25" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
       <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="11" t="s">
+      <c r="L25" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" s="9">
         <v>20</v>
       </c>
-      <c r="N25" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="O25" s="9">
+      <c r="O25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="P25" s="12" t="s">
-        <v>21</v>
-      </c>
+      <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
@@ -2675,9 +3332,8 @@
       <c r="AG25" s="1"/>
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
-      <c r="AJ25" s="1"/>
-    </row>
-    <row r="26" spans="1:36" ht="22" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:35" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="1"/>
       <c r="B26" s="23" t="s">
         <v>0</v>
@@ -2692,24 +3348,32 @@
         <v>3</v>
       </c>
       <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
+      <c r="G26" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>3</v>
+      </c>
       <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="N26" s="14" t="s">
+      <c r="L26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O26" s="14">
+      <c r="N26" s="14">
         <v>10</v>
       </c>
-      <c r="P26" s="15" t="s">
-        <v>43</v>
-      </c>
+      <c r="O26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="P26" s="1"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2729,12 +3393,11 @@
       <c r="AG26" s="1"/>
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
-      <c r="AJ26" s="1"/>
-    </row>
-    <row r="27" spans="1:36" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:35" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>9</v>
@@ -2743,19 +3406,27 @@
         <v>10</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="F27" s="6"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
+      <c r="G27" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H27" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="9">
+        <v>10</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
       <c r="O27" s="5"/>
-      <c r="P27" s="5"/>
+      <c r="P27" s="1"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2775,9 +3446,8 @@
       <c r="AG27" s="1"/>
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
-      <c r="AJ27" s="1"/>
-    </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="8" t="s">
         <v>12</v>
@@ -2789,19 +3459,27 @@
         <v>100</v>
       </c>
       <c r="E28" s="10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="G28" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="I28" s="30">
+        <v>100</v>
+      </c>
+      <c r="J28" s="31" t="s">
+        <v>75</v>
+      </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
       <c r="N28" s="5"/>
       <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -2821,12 +3499,11 @@
       <c r="AG28" s="1"/>
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
-      <c r="AJ28" s="1"/>
-    </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>4</v>
@@ -2835,19 +3512,19 @@
         <v>100</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
+      <c r="G29" s="36"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="36"/>
+      <c r="J29" s="36"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
       <c r="O29" s="5"/>
-      <c r="P29" s="5"/>
+      <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
@@ -2867,33 +3544,32 @@
       <c r="AG29" s="1"/>
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
-      <c r="AJ29" s="1"/>
-    </row>
-    <row r="30" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="20">
-        <v>12</v>
-      </c>
-      <c r="E30" s="21" t="s">
+      <c r="C30" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="9">
+        <v>8</v>
+      </c>
+      <c r="E30" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
-      <c r="P30" s="5"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
@@ -2913,25 +3589,32 @@
       <c r="AG30" s="1"/>
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
-      <c r="AJ30" s="1"/>
-    </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
-      <c r="E31" s="18"/>
+      <c r="B31" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="D31" s="30">
+        <v>10</v>
+      </c>
+      <c r="E31" s="31" t="s">
+        <v>64</v>
+      </c>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
       <c r="O31" s="5"/>
-      <c r="P31" s="5"/>
+      <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
@@ -2951,9 +3634,8 @@
       <c r="AG31" s="1"/>
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
-      <c r="AJ31" s="1"/>
-    </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2989,9 +3671,8 @@
       <c r="AG32" s="1"/>
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
-      <c r="AJ32" s="1"/>
-    </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -3027,9 +3708,8 @@
       <c r="AG33" s="1"/>
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
-      <c r="AJ33" s="1"/>
-    </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -3065,9 +3745,8 @@
       <c r="AG34" s="1"/>
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
-      <c r="AJ34" s="1"/>
-    </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -3103,9 +3782,8 @@
       <c r="AG35" s="1"/>
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
-      <c r="AJ35" s="1"/>
-    </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -3141,9 +3819,8 @@
       <c r="AG36" s="1"/>
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
-      <c r="AJ36" s="1"/>
-    </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -3179,9 +3856,8 @@
       <c r="AG37" s="1"/>
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
-      <c r="AJ37" s="1"/>
-    </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -3217,9 +3893,8 @@
       <c r="AG38" s="1"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
-      <c r="AJ38" s="1"/>
-    </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -3255,9 +3930,8 @@
       <c r="AG39" s="1"/>
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
-      <c r="AJ39" s="1"/>
-    </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -3293,9 +3967,8 @@
       <c r="AG40" s="1"/>
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
-      <c r="AJ40" s="1"/>
-    </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -3331,9 +4004,8 @@
       <c r="AG41" s="1"/>
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
-      <c r="AJ41" s="1"/>
-    </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -3369,9 +4041,8 @@
       <c r="AG42" s="1"/>
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
-      <c r="AJ42" s="1"/>
-    </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -3407,9 +4078,8 @@
       <c r="AG43" s="1"/>
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
-      <c r="AJ43" s="1"/>
-    </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -3445,9 +4115,8 @@
       <c r="AG44" s="1"/>
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
-      <c r="AJ44" s="1"/>
-    </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -3483,9 +4152,8 @@
       <c r="AG45" s="1"/>
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
-      <c r="AJ45" s="1"/>
-    </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -3521,9 +4189,8 @@
       <c r="AG46" s="1"/>
       <c r="AH46" s="1"/>
       <c r="AI46" s="1"/>
-      <c r="AJ46" s="1"/>
-    </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -3559,9 +4226,8 @@
       <c r="AG47" s="1"/>
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
-      <c r="AJ47" s="1"/>
-    </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -3597,9 +4263,8 @@
       <c r="AG48" s="1"/>
       <c r="AH48" s="1"/>
       <c r="AI48" s="1"/>
-      <c r="AJ48" s="1"/>
-    </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3635,9 +4300,8 @@
       <c r="AG49" s="1"/>
       <c r="AH49" s="1"/>
       <c r="AI49" s="1"/>
-      <c r="AJ49" s="1"/>
-    </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3673,9 +4337,8 @@
       <c r="AG50" s="1"/>
       <c r="AH50" s="1"/>
       <c r="AI50" s="1"/>
-      <c r="AJ50" s="1"/>
-    </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3711,9 +4374,8 @@
       <c r="AG51" s="1"/>
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
-      <c r="AJ51" s="1"/>
-    </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3749,9 +4411,8 @@
       <c r="AG52" s="1"/>
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
-      <c r="AJ52" s="1"/>
-    </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3787,9 +4448,8 @@
       <c r="AG53" s="1"/>
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
-      <c r="AJ53" s="1"/>
-    </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3825,9 +4485,8 @@
       <c r="AG54" s="1"/>
       <c r="AH54" s="1"/>
       <c r="AI54" s="1"/>
-      <c r="AJ54" s="1"/>
-    </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3863,9 +4522,8 @@
       <c r="AG55" s="1"/>
       <c r="AH55" s="1"/>
       <c r="AI55" s="1"/>
-      <c r="AJ55" s="1"/>
-    </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -3901,9 +4559,8 @@
       <c r="AG56" s="1"/>
       <c r="AH56" s="1"/>
       <c r="AI56" s="1"/>
-      <c r="AJ56" s="1"/>
-    </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -3939,9 +4596,8 @@
       <c r="AG57" s="1"/>
       <c r="AH57" s="1"/>
       <c r="AI57" s="1"/>
-      <c r="AJ57" s="1"/>
-    </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -3977,9 +4633,8 @@
       <c r="AG58" s="1"/>
       <c r="AH58" s="1"/>
       <c r="AI58" s="1"/>
-      <c r="AJ58" s="1"/>
-    </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -4015,9 +4670,8 @@
       <c r="AG59" s="1"/>
       <c r="AH59" s="1"/>
       <c r="AI59" s="1"/>
-      <c r="AJ59" s="1"/>
-    </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -4053,9 +4707,8 @@
       <c r="AG60" s="1"/>
       <c r="AH60" s="1"/>
       <c r="AI60" s="1"/>
-      <c r="AJ60" s="1"/>
-    </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -4091,9 +4744,8 @@
       <c r="AG61" s="1"/>
       <c r="AH61" s="1"/>
       <c r="AI61" s="1"/>
-      <c r="AJ61" s="1"/>
-    </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -4129,9 +4781,8 @@
       <c r="AG62" s="1"/>
       <c r="AH62" s="1"/>
       <c r="AI62" s="1"/>
-      <c r="AJ62" s="1"/>
-    </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -4167,9 +4818,8 @@
       <c r="AG63" s="1"/>
       <c r="AH63" s="1"/>
       <c r="AI63" s="1"/>
-      <c r="AJ63" s="1"/>
-    </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -4205,9 +4855,8 @@
       <c r="AG64" s="1"/>
       <c r="AH64" s="1"/>
       <c r="AI64" s="1"/>
-      <c r="AJ64" s="1"/>
-    </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -4243,9 +4892,8 @@
       <c r="AG65" s="1"/>
       <c r="AH65" s="1"/>
       <c r="AI65" s="1"/>
-      <c r="AJ65" s="1"/>
-    </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -4281,9 +4929,8 @@
       <c r="AG66" s="1"/>
       <c r="AH66" s="1"/>
       <c r="AI66" s="1"/>
-      <c r="AJ66" s="1"/>
-    </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -4319,9 +4966,8 @@
       <c r="AG67" s="1"/>
       <c r="AH67" s="1"/>
       <c r="AI67" s="1"/>
-      <c r="AJ67" s="1"/>
-    </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -4357,9 +5003,8 @@
       <c r="AG68" s="1"/>
       <c r="AH68" s="1"/>
       <c r="AI68" s="1"/>
-      <c r="AJ68" s="1"/>
-    </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -4395,9 +5040,8 @@
       <c r="AG69" s="1"/>
       <c r="AH69" s="1"/>
       <c r="AI69" s="1"/>
-      <c r="AJ69" s="1"/>
-    </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -4433,9 +5077,8 @@
       <c r="AG70" s="1"/>
       <c r="AH70" s="1"/>
       <c r="AI70" s="1"/>
-      <c r="AJ70" s="1"/>
-    </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -4471,9 +5114,8 @@
       <c r="AG71" s="1"/>
       <c r="AH71" s="1"/>
       <c r="AI71" s="1"/>
-      <c r="AJ71" s="1"/>
-    </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -4509,9 +5151,8 @@
       <c r="AG72" s="1"/>
       <c r="AH72" s="1"/>
       <c r="AI72" s="1"/>
-      <c r="AJ72" s="1"/>
-    </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -4547,9 +5188,8 @@
       <c r="AG73" s="1"/>
       <c r="AH73" s="1"/>
       <c r="AI73" s="1"/>
-      <c r="AJ73" s="1"/>
-    </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -4585,9 +5225,8 @@
       <c r="AG74" s="1"/>
       <c r="AH74" s="1"/>
       <c r="AI74" s="1"/>
-      <c r="AJ74" s="1"/>
-    </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -4623,9 +5262,8 @@
       <c r="AG75" s="1"/>
       <c r="AH75" s="1"/>
       <c r="AI75" s="1"/>
-      <c r="AJ75" s="1"/>
-    </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -4661,9 +5299,8 @@
       <c r="AG76" s="1"/>
       <c r="AH76" s="1"/>
       <c r="AI76" s="1"/>
-      <c r="AJ76" s="1"/>
-    </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -4699,9 +5336,8 @@
       <c r="AG77" s="1"/>
       <c r="AH77" s="1"/>
       <c r="AI77" s="1"/>
-      <c r="AJ77" s="1"/>
-    </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -4737,9 +5373,8 @@
       <c r="AG78" s="1"/>
       <c r="AH78" s="1"/>
       <c r="AI78" s="1"/>
-      <c r="AJ78" s="1"/>
-    </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -4775,9 +5410,8 @@
       <c r="AG79" s="1"/>
       <c r="AH79" s="1"/>
       <c r="AI79" s="1"/>
-      <c r="AJ79" s="1"/>
-    </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -4813,9 +5447,8 @@
       <c r="AG80" s="1"/>
       <c r="AH80" s="1"/>
       <c r="AI80" s="1"/>
-      <c r="AJ80" s="1"/>
-    </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -4851,9 +5484,8 @@
       <c r="AG81" s="1"/>
       <c r="AH81" s="1"/>
       <c r="AI81" s="1"/>
-      <c r="AJ81" s="1"/>
-    </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -4889,9 +5521,8 @@
       <c r="AG82" s="1"/>
       <c r="AH82" s="1"/>
       <c r="AI82" s="1"/>
-      <c r="AJ82" s="1"/>
-    </row>
-    <row r="83" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -4927,9 +5558,8 @@
       <c r="AG83" s="1"/>
       <c r="AH83" s="1"/>
       <c r="AI83" s="1"/>
-      <c r="AJ83" s="1"/>
-    </row>
-    <row r="84" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -4965,9 +5595,8 @@
       <c r="AG84" s="1"/>
       <c r="AH84" s="1"/>
       <c r="AI84" s="1"/>
-      <c r="AJ84" s="1"/>
-    </row>
-    <row r="85" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -5003,9 +5632,8 @@
       <c r="AG85" s="1"/>
       <c r="AH85" s="1"/>
       <c r="AI85" s="1"/>
-      <c r="AJ85" s="1"/>
-    </row>
-    <row r="86" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -5041,9 +5669,8 @@
       <c r="AG86" s="1"/>
       <c r="AH86" s="1"/>
       <c r="AI86" s="1"/>
-      <c r="AJ86" s="1"/>
-    </row>
-    <row r="87" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -5079,9 +5706,8 @@
       <c r="AG87" s="1"/>
       <c r="AH87" s="1"/>
       <c r="AI87" s="1"/>
-      <c r="AJ87" s="1"/>
-    </row>
-    <row r="88" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -5117,9 +5743,8 @@
       <c r="AG88" s="1"/>
       <c r="AH88" s="1"/>
       <c r="AI88" s="1"/>
-      <c r="AJ88" s="1"/>
-    </row>
-    <row r="89" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -5155,9 +5780,8 @@
       <c r="AG89" s="1"/>
       <c r="AH89" s="1"/>
       <c r="AI89" s="1"/>
-      <c r="AJ89" s="1"/>
-    </row>
-    <row r="90" spans="1:36" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -5193,10 +5817,10 @@
       <c r="AG90" s="1"/>
       <c r="AH90" s="1"/>
       <c r="AI90" s="1"/>
-      <c r="AJ90" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>